<commit_message>
env 7010 update test objects to follow global variable
</commit_message>
<xml_diff>
--- a/testdatacollections.xlsx
+++ b/testdatacollections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultant_MSPHitect\Documents\1SPEK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultant_MSPHitect\Katalon Studio\TrainingonKatalon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182D95C6-D131-4F12-8B69-D7585E43DA98}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382D3C71-9D86-4B3C-9076-49B06AF76C71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="2196" windowWidth="14400" windowHeight="7440" xr2:uid="{5EDC348E-6822-4A81-98BC-4DFC952AB5D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EDC348E-6822-4A81-98BC-4DFC952AB5D7}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Amaun(RM)</t>
+  </si>
+  <si>
+    <t>PTJ</t>
   </si>
 </sst>
 </file>
@@ -462,28 +465,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD3ECCB-B8C3-4AD3-BB52-27FBF1F4DB89}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
     <col min="2" max="2" width="30.21875" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>790214108888</v>
       </c>
@@ -491,7 +497,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>601101955194</v>
       </c>
@@ -499,7 +505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>112233445566</v>
       </c>
@@ -507,27 +513,43 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>810213016116</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>600803015724</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>820806015126</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>780613015177</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>

</xml_diff>

<commit_message>
update for 7010 object repo
</commit_message>
<xml_diff>
--- a/testdatacollections.xlsx
+++ b/testdatacollections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultant_MSPHitect\Katalon Studio\TrainingonKatalon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382D3C71-9D86-4B3C-9076-49B06AF76C71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B4351-BDE5-419A-9CA3-1B7D849017B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EDC348E-6822-4A81-98BC-4DFC952AB5D7}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update PT with cara bayaran EFT for 7010
</commit_message>
<xml_diff>
--- a/testdatacollections.xlsx
+++ b/testdatacollections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultant_MSPHitect\Katalon Studio\TrainingonKatalon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B4351-BDE5-419A-9CA3-1B7D849017B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E106FC7-909E-4BF4-AC3B-8E8785C57C07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EDC348E-6822-4A81-98BC-4DFC952AB5D7}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>600803015724</v>
+        <v>860828665169</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
7011 and 7010 complete with 8 processes
</commit_message>
<xml_diff>
--- a/testdatacollections.xlsx
+++ b/testdatacollections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultant_MSPHitect\Katalon Studio\TrainingonKatalon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E106FC7-909E-4BF4-AC3B-8E8785C57C07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996AB77-2D96-454B-8453-DFB4ED825BAD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5EDC348E-6822-4A81-98BC-4DFC952AB5D7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -468,7 +468,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,8 +546,12 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="1">
+        <v>780613015177</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>

</xml_diff>